<commit_message>
Make rw-fast-excel version 2
</commit_message>
<xml_diff>
--- a/src/main/resources/simple.xlsx
+++ b/src/main/resources/simple.xlsx
@@ -167,13 +167,10 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.562962962963"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>